<commit_message>
Player의 Original Data를 Firebase에 업로드하는 코드 추가
</commit_message>
<xml_diff>
--- a/RhythmiCar_Unity/Assets/Resources/Data/DataBase.xlsx
+++ b/RhythmiCar_Unity/Assets/Resources/Data/DataBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HSH\Documents\Rhythm\RhythmiCar_Unity\Assets\Resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6EC22E0-A2EF-4AAD-97A3-E283C721415A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB997783-C2D0-4AEF-A896-870AEAF41549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3585" yWindow="2850" windowWidth="12090" windowHeight="7905" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3585" yWindow="2850" windowWidth="12090" windowHeight="7905" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CarData" sheetId="1" r:id="rId1"/>
@@ -401,10 +401,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>_196BPM_Bluedy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>WakeUp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -439,6 +435,9 @@
   <si>
     <t>MaxSpeed</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_196BPM_SuddenShower</t>
   </si>
 </sst>
 </file>
@@ -2333,8 +2332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E72EDC-E801-451A-A818-5D9F5732F12C}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2359,16 +2358,16 @@
         <v>18</v>
       </c>
       <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>31</v>
-      </c>
-      <c r="G1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2376,10 +2375,10 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -2399,10 +2398,10 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -2422,10 +2421,10 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
         <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -2442,13 +2441,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -2474,7 +2473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C077E246-CD85-420D-A5E6-48AAD0E5E620}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -2482,13 +2481,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>